<commit_message>
feature/54601 = update UI/UX my timesheet, expand column when click, add required icon
</commit_message>
<xml_diff>
--- a/aspnet-core/src/Timesheet.Web.Host/wwwroot/template/ExportTeamWorkingCalender.xlsx
+++ b/aspnet-core/src/Timesheet.Web.Host/wwwroot/template/ExportTeamWorkingCalender.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ncc-erp-timesheet\aspnet-core\src\Timesheet.Web.Host\wwwroot\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AB5FA9-4FFB-4905-B8EE-290520D16C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4989B3C2-F4CA-49D4-9B5E-0936375F5144}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,8 +65,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +81,22 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -105,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -114,6 +129,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,27 +446,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4E0E3B-86D6-43B6-AF29-18792EF63F26}">
-  <dimension ref="A3:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I3" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -475,7 +516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -486,6 +527,9 @@
       <c r="H4" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feature/54622 = Improve team working calendar performance, update export data team working calendar
</commit_message>
<xml_diff>
--- a/aspnet-core/src/Timesheet.Web.Host/wwwroot/template/ExportTeamWorkingCalender.xlsx
+++ b/aspnet-core/src/Timesheet.Web.Host/wwwroot/template/ExportTeamWorkingCalender.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ncc-erp-timesheet\aspnet-core\src\Timesheet.Web.Host\wwwroot\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NCC\ncc-erp-timesheet\aspnet-core\src\Timesheet.Web.Host\wwwroot\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>User Name</t>
   </si>
@@ -60,13 +60,16 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +102,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,10 +140,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,76 +461,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I1:I1048576"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="1" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -525,10 +544,11 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>